<commit_message>
Update canonical resolution list
</commit_message>
<xml_diff>
--- a/Medicare-Records-FHIR-IG-redirects.xlsx
+++ b/Medicare-Records-FHIR-IG-redirects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\ci-medicare-records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFAE3B1-EA5C-47A2-925A-BFACD2EA7152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4082E98-7D9D-4981-966E-856AFF0BD677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FBD9E2B4-3F0E-45D9-8508-0EDB941B2BB2}"/>
+    <workbookView xWindow="-24195" yWindow="1335" windowWidth="21600" windowHeight="14550" activeTab="1" xr2:uid="{FBD9E2B4-3F0E-45D9-8508-0EDB941B2BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Publication redirects" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Publication Redirections</t>
   </si>
@@ -91,39 +91,6 @@
     <t>https://developer.digitalhealth.gov.au/sites/default/files/specifications/clinical-documents/ep-2746-2018/dh-2738-2018/index.html</t>
   </si>
   <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/immunization-air/2.1.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/flag-air-1/2.1.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/consent-aodr/2.1.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/bodysite-aodr/2.1.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/explanationofbenefit-medicare/2.1.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/referralrequest-mbsdva/2.1.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/medicationrequest-pbs/2.1.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/medication-pbs/2.1.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/extension-donationdecision/2.1.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/extension-dateinitialregistration/2.1.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/vaccine-serial-number-1/2.1.0</t>
-  </si>
-  <si>
     <t>http://ns.electronichealth.net.au/fhir/medicare-records</t>
   </si>
   <si>
@@ -136,33 +103,6 @@
     <t>http://ns.electronichealth.net.au/fhir/medicare-records/package.tgz</t>
   </si>
   <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/immunization-air/2.2.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/flag-air-1/2.2.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/consent-aodr/2.2.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/bodysite-aodr/2.2.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/explanationofbenefit-medicare/2.2.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/medicationrequest-pbs/2.2.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/medication-pbs/2.2.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/extension-donationdecision/2.2.0</t>
-  </si>
-  <si>
-    <t>http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/vaccine-serial-number-1/2.2.0</t>
-  </si>
-  <si>
     <t>N/A - profile does not exist in latest version of Medicare Records (2.2.0)</t>
   </si>
   <si>
@@ -208,88 +148,28 @@
     <t>https://fhir.digitalhealth.gov.au/dh/StructureDefinition-dh-immunization-air.html</t>
   </si>
   <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-immunization-air.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.2.0/StructureDefinition-dh-immunization-air.html</t>
-  </si>
-  <si>
     <t>https://fhir.digitalhealth.gov.au/dh/StructureDefinition-dh-flag-air-1.html</t>
   </si>
   <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-flag-air-1.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.2.0/StructureDefinition-dh-flag-air-1.html</t>
-  </si>
-  <si>
     <t>https://fhir.digitalhealth.gov.au/dh/StructureDefinition-dh-consent-aodr.html</t>
   </si>
   <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-consent-aodr.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.2.0/StructureDefinition-dh-consent-aodr.html</t>
-  </si>
-  <si>
     <t>https://fhir.digitalhealth.gov.au/dh/StructureDefinition-dh-bodysite-aodr.html</t>
   </si>
   <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-bodysite-aodr.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.2.0/StructureDefinition-dh-bodysite-aodr.html</t>
-  </si>
-  <si>
     <t>https://fhir.digitalhealth.gov.au/dh/StructureDefinition-dh-explanationofbenefit-medicare.html</t>
   </si>
   <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-explanationofbenefit-medicare.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.2.0/StructureDefinition-dh-explanationofbenefit-medicare.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-referralrequest-mbsdva.html</t>
-  </si>
-  <si>
     <t>https://fhir.digitalhealth.gov.au/dh/StructureDefinition-dh-medicationrequest-pbs.html</t>
   </si>
   <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-medicationrequest-pbs.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.2.0/StructureDefinition-dh-medicationrequest-pbs.html</t>
-  </si>
-  <si>
     <t>https://fhir.digitalhealth.gov.au/dh/StructureDefinition-dh-medication-pbs.html</t>
   </si>
   <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-medication-pbs.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.2.0/StructureDefinition-dh-medication-pbs.html</t>
-  </si>
-  <si>
     <t>https://fhir.digitalhealth.gov.au/dh/StructureDefinition-dh-extension-donationdecision.html</t>
   </si>
   <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-extension-donationdecision.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.2.0/StructureDefinition-dh-extension-donationdecision.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-extension-dateinitialregistration.html</t>
-  </si>
-  <si>
     <t>https://fhir.digitalhealth.gov.au/dh/StructureDefinition-dh-vaccine-serial-number-1.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.1.0/StructureDefinition-dh-vaccine-serial-number-1.html</t>
-  </si>
-  <si>
-    <t>https://fhir.digitalhealth.gov.au/STU3/medicare-records/2.2.0/StructureDefinition-dh-vaccine-serial-number-1.html</t>
   </si>
 </sst>
 </file>
@@ -369,13 +249,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -702,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E66D00-41CA-49CD-903D-771BF0BACE39}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,75 +605,75 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>46</v>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>48</v>
+      <c r="A6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>50</v>
+      <c r="A7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>52</v>
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>48</v>
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>53</v>
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>54</v>
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>55</v>
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -822,10 +701,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FBC8FD9-F5CD-4A7B-86B9-827957D6BB68}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,357 +727,160 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>46</v>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>84</v>
-      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B19">
+    <sortCondition ref="A5:A19"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="A14" r:id="rId1" xr:uid="{4F93D6EB-D712-4CDB-B0A8-4E6FB4E0C857}"/>
-    <hyperlink ref="A21" r:id="rId2" xr:uid="{EE38274D-3C18-4289-BFDA-7762AAE8EAF1}"/>
-    <hyperlink ref="A28" r:id="rId3" xr:uid="{36A12DA2-B96F-4C26-9DFD-C4EB23BFF63D}"/>
-    <hyperlink ref="B10" r:id="rId4" xr:uid="{8BE1604E-00AB-4555-B209-1309C37B603F}"/>
-    <hyperlink ref="B13" r:id="rId5" xr:uid="{281D70BE-4021-43A8-9443-F46CA7866884}"/>
-    <hyperlink ref="B16" r:id="rId6" xr:uid="{790685CD-3A22-4F88-95A7-2AE20785A20D}"/>
-    <hyperlink ref="B19" r:id="rId7" xr:uid="{0C383A7B-D55E-4F3B-A5D9-F83D6A70AC67}"/>
-    <hyperlink ref="B22" r:id="rId8" xr:uid="{41BDEC43-C6D6-4C5B-B003-D60C1952341D}"/>
-    <hyperlink ref="B25" r:id="rId9" xr:uid="{0EDE2047-E0FC-43AF-8C53-D9380CBD782C}"/>
-    <hyperlink ref="B27" r:id="rId10" xr:uid="{AEEB4835-584F-42DE-B5F7-77710E17837E}"/>
-    <hyperlink ref="B30" r:id="rId11" display="https://www.digitalhealth.gov.au/fhir/STU3/medicare-records/2.1.0/StructureDefinition-dh-medication-pbs.html" xr:uid="{BD414888-0906-42DD-B0E9-DC7AEC731155}"/>
-    <hyperlink ref="B33" r:id="rId12" xr:uid="{83393932-F6E7-4710-BFAC-5362A5C8B228}"/>
-    <hyperlink ref="B36" r:id="rId13" xr:uid="{B5B7D40C-928A-4CDE-9F46-8586922C0698}"/>
-    <hyperlink ref="B38" r:id="rId14" display="https://www.digitalhealth.gov.au/fhir/STU3/medicare-records/2.1.0/StructureDefinition-dh-vaccine-serial-number-1.html" xr:uid="{515E94FF-992E-45D2-8E05-946A183E1B8C}"/>
-    <hyperlink ref="B11" r:id="rId15" xr:uid="{7D5FA91E-AC68-475D-8B3A-BBDEDD59F924}"/>
-    <hyperlink ref="B14" r:id="rId16" xr:uid="{E9693161-03CF-4457-A45B-5C627CD406E4}"/>
-    <hyperlink ref="B17" r:id="rId17" xr:uid="{9F25F842-9AFD-45C6-A52F-2EBF77E46807}"/>
-    <hyperlink ref="B20" r:id="rId18" xr:uid="{8833BF99-969D-4001-951A-CBE3D629710E}"/>
-    <hyperlink ref="B23" r:id="rId19" xr:uid="{0A58B9A9-9510-4383-B2F3-4129B787E2E2}"/>
-    <hyperlink ref="B28" r:id="rId20" xr:uid="{B0C5517A-A8A5-4B76-9CA3-8924E2C93D64}"/>
-    <hyperlink ref="B31" r:id="rId21" xr:uid="{2D7B84AD-09BE-454A-AEB0-D357AB424659}"/>
-    <hyperlink ref="B34" r:id="rId22" xr:uid="{76939DF3-AD83-4240-A7B3-C1558DBBA85D}"/>
-    <hyperlink ref="B39" r:id="rId23" xr:uid="{54D6CB2A-69D9-43EF-BEE5-AAFA779E9BA4}"/>
-    <hyperlink ref="A10" r:id="rId24" xr:uid="{D2812E50-7EB2-4FBB-82EE-117F3F5B2BE4}"/>
-    <hyperlink ref="A9" r:id="rId25" xr:uid="{A7F81444-D909-4145-8493-2850105ECE1C}"/>
-    <hyperlink ref="A13" r:id="rId26" xr:uid="{3FC4C19A-3D04-4EFA-A488-3E0EB72989C7}"/>
-    <hyperlink ref="A12" r:id="rId27" xr:uid="{C631BBD6-D9AC-461B-A2B7-8B43580EFA7B}"/>
-    <hyperlink ref="A15" r:id="rId28" xr:uid="{53E1B9C1-6EE0-4B6C-B528-897C628467DB}"/>
-    <hyperlink ref="A16" r:id="rId29" xr:uid="{1F31E231-4C41-44F3-BBF2-E9D0EA6A4F63}"/>
-    <hyperlink ref="A18" r:id="rId30" xr:uid="{6D9768A7-FB3E-4D89-AC50-59A8D236CB68}"/>
-    <hyperlink ref="A19" r:id="rId31" xr:uid="{42ED265C-49DC-4727-ADF5-6A6F9666D95D}"/>
-    <hyperlink ref="A22" r:id="rId32" xr:uid="{52AAD81A-5CDF-4032-BCD1-E989238AACA8}"/>
-    <hyperlink ref="A24" r:id="rId33" xr:uid="{7197E7F5-7CBF-4550-88F9-18E69F1F03A8}"/>
-    <hyperlink ref="A25" r:id="rId34" xr:uid="{E3793B82-A9E6-4B45-B0AC-558E45AC793B}"/>
-    <hyperlink ref="A27" r:id="rId35" xr:uid="{972922E0-7CBD-4E88-9F55-FB5B78F0E256}"/>
-    <hyperlink ref="A29" r:id="rId36" xr:uid="{50585E08-DD84-422A-BA1B-6D9D8D0AABDB}"/>
-    <hyperlink ref="A30" r:id="rId37" xr:uid="{41ED08EB-73F8-415F-A193-C2E4303C9C09}"/>
-    <hyperlink ref="A32" r:id="rId38" xr:uid="{B27B2471-ED38-4ECF-9732-4B3AFBA2B174}"/>
-    <hyperlink ref="A33" r:id="rId39" xr:uid="{DF83E3DD-1F5D-423B-85E1-9C8EA49196B4}"/>
-    <hyperlink ref="A35" r:id="rId40" xr:uid="{B86A2DF9-C44E-4C01-8974-82731FC370CA}"/>
-    <hyperlink ref="A36" r:id="rId41" xr:uid="{23901E94-7360-49C7-9309-84B8A9F2E899}"/>
-    <hyperlink ref="A37" r:id="rId42" xr:uid="{F44C1C32-4DAF-4C10-A0BA-B03F9CB69BAC}"/>
-    <hyperlink ref="A38" r:id="rId43" xr:uid="{44F11E14-ECDF-4A87-A21A-0F764D1C0D60}"/>
-    <hyperlink ref="A11" r:id="rId44" xr:uid="{751F8E52-EF25-4E7E-9B1F-0D2D77DE3EFC}"/>
-    <hyperlink ref="A17" r:id="rId45" xr:uid="{956ECAB3-813F-4A86-A409-B562493A2481}"/>
-    <hyperlink ref="A20" r:id="rId46" xr:uid="{3CDD7B06-46A0-45CB-A9B6-CAF707682671}"/>
-    <hyperlink ref="A23" r:id="rId47" xr:uid="{41A8A4DD-417F-4E89-9394-2987A9CA3F3E}"/>
-    <hyperlink ref="A26" r:id="rId48" xr:uid="{DFEE65BE-FA71-45C2-BC1E-83E16C51EDBB}"/>
-    <hyperlink ref="A31" r:id="rId49" xr:uid="{4D73F5A2-A11A-443B-A661-CD6BE72AA2B3}"/>
-    <hyperlink ref="A34" r:id="rId50" xr:uid="{EB242800-4C53-4086-9487-6EE3234E99BE}"/>
-    <hyperlink ref="A39" r:id="rId51" xr:uid="{1BAAB6E9-97CC-49B4-8494-C69BD40FC559}"/>
-    <hyperlink ref="B9" r:id="rId52" xr:uid="{E546F323-923B-4316-A04A-6CE5E59F4D54}"/>
-    <hyperlink ref="B12" r:id="rId53" xr:uid="{B0C02055-19DB-4038-AA46-0A2112C2D387}"/>
-    <hyperlink ref="B15" r:id="rId54" xr:uid="{7905CEE5-D0EC-44A8-98BA-C3DD199DFFD2}"/>
-    <hyperlink ref="B18" r:id="rId55" xr:uid="{864FF5A3-BA49-4DCC-9AAB-A56929D176F6}"/>
-    <hyperlink ref="B21" r:id="rId56" xr:uid="{48E73D4E-0DAD-4EA5-A65A-533919E6D6A2}"/>
-    <hyperlink ref="B24" r:id="rId57" display="https://www.digitalhealth.gov.au/fhir/dh/StructureDefinition-dh-referralrequest-mbsdva.html" xr:uid="{65A0A886-797F-4DC9-83F6-57E2F5C5206C}"/>
-    <hyperlink ref="B26" r:id="rId58" xr:uid="{DDC2A63A-285A-491E-A22C-B4FBC2F4AE48}"/>
-    <hyperlink ref="B29" r:id="rId59" xr:uid="{BFAFCCD1-2106-4676-BE12-A50ACD3AE9A6}"/>
-    <hyperlink ref="B32" r:id="rId60" display="https://www.digitalhealth.gov.au/fhir/dh/StructureDefinition-dh-extension-donationdecision.html" xr:uid="{232B8F73-AEA2-4794-9760-28C32F0489D4}"/>
-    <hyperlink ref="B35" r:id="rId61" display="https://www.digitalhealth.gov.au/fhir/dh/StructureDefinition-dh-referralrequest-mbsdva.html" xr:uid="{9DEE84C8-C67B-4563-AD54-54DFB360B1D9}"/>
-    <hyperlink ref="B37" r:id="rId62" xr:uid="{379AC3D9-611B-45AC-A281-BB65B5A29967}"/>
-    <hyperlink ref="A8" r:id="rId63" xr:uid="{2F7EAA36-628C-442F-B49B-0069128E5F97}"/>
-    <hyperlink ref="A7" r:id="rId64" xr:uid="{4001DC7D-82E5-4154-9DD7-596F0E5449C4}"/>
-    <hyperlink ref="A6" r:id="rId65" xr:uid="{347A5577-F73F-4E85-B616-C7D0A05EFD5C}"/>
-    <hyperlink ref="B6" r:id="rId66" xr:uid="{77D6B49D-24D1-4D4E-8CAB-F20AFABD927C}"/>
-    <hyperlink ref="B7" r:id="rId67" xr:uid="{85211D0D-4A48-470A-A909-7E7F36C32C04}"/>
-    <hyperlink ref="B8" r:id="rId68" xr:uid="{C68B401A-1F58-4B38-800F-AC373E815609}"/>
+    <hyperlink ref="A11" r:id="rId1" xr:uid="{EE38274D-3C18-4289-BFDA-7762AAE8EAF1}"/>
+    <hyperlink ref="A15" r:id="rId2" xr:uid="{A7F81444-D909-4145-8493-2850105ECE1C}"/>
+    <hyperlink ref="A14" r:id="rId3" xr:uid="{C631BBD6-D9AC-461B-A2B7-8B43580EFA7B}"/>
+    <hyperlink ref="A10" r:id="rId4" xr:uid="{53E1B9C1-6EE0-4B6C-B528-897C628467DB}"/>
+    <hyperlink ref="A9" r:id="rId5" xr:uid="{6D9768A7-FB3E-4D89-AC50-59A8D236CB68}"/>
+    <hyperlink ref="A18" r:id="rId6" xr:uid="{7197E7F5-7CBF-4550-88F9-18E69F1F03A8}"/>
+    <hyperlink ref="A16" r:id="rId7" xr:uid="{50585E08-DD84-422A-BA1B-6D9D8D0AABDB}"/>
+    <hyperlink ref="A13" r:id="rId8" xr:uid="{B27B2471-ED38-4ECF-9732-4B3AFBA2B174}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{B86A2DF9-C44E-4C01-8974-82731FC370CA}"/>
+    <hyperlink ref="A19" r:id="rId10" xr:uid="{F44C1C32-4DAF-4C10-A0BA-B03F9CB69BAC}"/>
+    <hyperlink ref="A17" r:id="rId11" xr:uid="{DFEE65BE-FA71-45C2-BC1E-83E16C51EDBB}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{E546F323-923B-4316-A04A-6CE5E59F4D54}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{B0C02055-19DB-4038-AA46-0A2112C2D387}"/>
+    <hyperlink ref="B10" r:id="rId14" xr:uid="{7905CEE5-D0EC-44A8-98BA-C3DD199DFFD2}"/>
+    <hyperlink ref="B9" r:id="rId15" xr:uid="{864FF5A3-BA49-4DCC-9AAB-A56929D176F6}"/>
+    <hyperlink ref="B11" r:id="rId16" xr:uid="{48E73D4E-0DAD-4EA5-A65A-533919E6D6A2}"/>
+    <hyperlink ref="B18" r:id="rId17" display="https://www.digitalhealth.gov.au/fhir/dh/StructureDefinition-dh-referralrequest-mbsdva.html" xr:uid="{65A0A886-797F-4DC9-83F6-57E2F5C5206C}"/>
+    <hyperlink ref="B17" r:id="rId18" xr:uid="{DDC2A63A-285A-491E-A22C-B4FBC2F4AE48}"/>
+    <hyperlink ref="B16" r:id="rId19" xr:uid="{BFAFCCD1-2106-4676-BE12-A50ACD3AE9A6}"/>
+    <hyperlink ref="B13" r:id="rId20" display="https://www.digitalhealth.gov.au/fhir/dh/StructureDefinition-dh-extension-donationdecision.html" xr:uid="{232B8F73-AEA2-4794-9760-28C32F0489D4}"/>
+    <hyperlink ref="B12" r:id="rId21" display="https://www.digitalhealth.gov.au/fhir/dh/StructureDefinition-dh-referralrequest-mbsdva.html" xr:uid="{9DEE84C8-C67B-4563-AD54-54DFB360B1D9}"/>
+    <hyperlink ref="B19" r:id="rId22" xr:uid="{379AC3D9-611B-45AC-A281-BB65B5A29967}"/>
+    <hyperlink ref="A6" r:id="rId23" xr:uid="{347A5577-F73F-4E85-B616-C7D0A05EFD5C}"/>
+    <hyperlink ref="B6" r:id="rId24" xr:uid="{77D6B49D-24D1-4D4E-8CAB-F20AFABD927C}"/>
+    <hyperlink ref="A7" r:id="rId25" xr:uid="{329917FB-086E-4586-AAAE-3BFFFF775F8B}"/>
+    <hyperlink ref="A8" r:id="rId26" xr:uid="{16877242-C245-4A2B-BB26-D2F214617FE4}"/>
+    <hyperlink ref="B7" r:id="rId27" xr:uid="{039B10FA-FFC2-4497-9586-ECA16F54CF36}"/>
+    <hyperlink ref="B8" r:id="rId28" xr:uid="{89D92095-3C09-48F0-8411-A9509F70D07D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId69"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>